<commit_message>
Agregué el nombre del director actual en el caso de la vista de exportación de reconocimientos en word
</commit_message>
<xml_diff>
--- a/Gestion_de_Cursos/Sistema/informacion_modificable/info.xlsx
+++ b/Gestion_de_Cursos/Sistema/informacion_modificable/info.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Director:</t>
   </si>
@@ -54,6 +54,15 @@
   </si>
   <si>
     <t>Sebas</t>
+  </si>
+  <si>
+    <t>Samuel Villanueva Aguero</t>
+  </si>
+  <si>
+    <t>Maritza Flores Sarabia</t>
+  </si>
+  <si>
+    <t>Andrea Jacqueline Burgos Perea</t>
   </si>
 </sst>
 </file>
@@ -105,7 +114,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="24.98046875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="7.18359375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -113,7 +122,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -121,7 +130,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -129,7 +138,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
@@ -145,7 +154,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>125.0</v>
+        <v>500.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eri: quiete la 's' que habia agregado de registros ahora ya esta como registro para que funcione Sebas: deba haber por lo menos 1 archivo en el directorio de importados y debe existir el archivo info con la hoja del año actual para que se habiliten los otros botones Denis: solo le modifique lo del formato de redireccionar le quite las fotos feas, y pues ya tiene los combos
</commit_message>
<xml_diff>
--- a/Gestion_de_Cursos/Sistema/informacion_modificable/info.xlsx
+++ b/Gestion_de_Cursos/Sistema/informacion_modificable/info.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Director:</t>
   </si>
@@ -56,13 +56,13 @@
     <t>Periodo Agosto-Diciembre:</t>
   </si>
   <si>
-    <t>dddddddddddd</t>
-  </si>
-  <si>
-    <t>jjjjjjjjjjjjjjjjjjjjjjj</t>
-  </si>
-  <si>
-    <t>ccccccccccccccc</t>
+    <t>direc</t>
+  </si>
+  <si>
+    <t>jefe</t>
+  </si>
+  <si>
+    <t>coo</t>
   </si>
 </sst>
 </file>
@@ -142,7 +142,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>87.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
@@ -150,7 +150,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
@@ -158,7 +158,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
@@ -166,7 +166,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
@@ -174,7 +174,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="9">
@@ -182,7 +182,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="10">
@@ -190,7 +190,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="11">
@@ -198,7 +198,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="12">
@@ -206,7 +206,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="13">
@@ -214,7 +214,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="n">
-        <v>452.0</v>
+        <v>80.0</v>
       </c>
     </row>
     <row r="14">
@@ -222,7 +222,7 @@
         <v>5</v>
       </c>
       <c r="B14" t="n">
-        <v>67.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="15">
@@ -230,7 +230,7 @@
         <v>6</v>
       </c>
       <c r="B15" t="n">
-        <v>55.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="16">
@@ -238,7 +238,7 @@
         <v>7</v>
       </c>
       <c r="B16" t="n">
-        <v>55.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="17">
@@ -246,7 +246,7 @@
         <v>8</v>
       </c>
       <c r="B17" t="n">
-        <v>55.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="18">
@@ -254,7 +254,7 @@
         <v>9</v>
       </c>
       <c r="B18" t="n">
-        <v>55.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="19">
@@ -262,7 +262,7 @@
         <v>10</v>
       </c>
       <c r="B19" t="n">
-        <v>55.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="20">
@@ -270,7 +270,7 @@
         <v>11</v>
       </c>
       <c r="B20" t="n">
-        <v>55.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="21">
@@ -278,7 +278,7 @@
         <v>12</v>
       </c>
       <c r="B21" t="n">
-        <v>55.0</v>
+        <v>10.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>